<commit_message>
Re-organized the repo so it's easier to find what you need
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Jan 2008 (Sample)" sheetId="2" r:id="rId1"/>
-    <sheet name="RAW DATA" sheetId="3" r:id="rId2"/>
+    <sheet name="Formatted Data Template" sheetId="2" r:id="rId1"/>
+    <sheet name="Raw Data Example" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Jan_2008_test_2" localSheetId="1">'Raw Data Example'!$A$1:$C$46</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -133,8 +136,82 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>User</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This equation allows you to match the ID's with the respective LOC count without manually matching them up yourself</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This table must be tabulated like this to get the look up to work.
+Use Ctrl+c, the right-click to see the paste options. One of them makes rows columns.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="Jan_2008_test1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\User\Documents\seng403_New\Jan_2008_test.txt" space="1" comma="1" consecutive="1" delimiter=":">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t xml:space="preserve">Contributor Name </t>
   </si>
@@ -177,12 +254,81 @@
   <si>
     <t>GHTorrentName</t>
   </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Dwight</t>
+  </si>
+  <si>
+    <t>a518f23a2b8b2a4499113b20057c76824ed5d1ac</t>
+  </si>
+  <si>
+    <t>db/</t>
+  </si>
+  <si>
+    <t>eef739da55fbab471e5adc76c1c7d5af0409499c</t>
+  </si>
+  <si>
+    <t>9e1d56bdd0c45deede6f1aeddfe40ee7817b50cb</t>
+  </si>
+  <si>
+    <t>5795cee2f7b12d5da89f0ec565409dbaed30a5af</t>
+  </si>
+  <si>
+    <t>093b76717eacaac4f51ec00ca67df911d8c64210</t>
+  </si>
+  <si>
+    <t>9f35516beb3b2df345022a9e97b163d7934ac635</t>
+  </si>
+  <si>
+    <t>a3d1609506773c9c67cc2950371dd149d7f0ca4b</t>
+  </si>
+  <si>
+    <t>b9c78504dbd7d05cf93b02f2bd28d3176184e35e</t>
+  </si>
+  <si>
+    <t>e20c9d2b0df280bf3742af2b5b671a008c108436</t>
+  </si>
+  <si>
+    <t>573b11ecd4c9592f4199f9c6f416a372e540765e</t>
+  </si>
+  <si>
+    <t>da8ecf472130fa901330d34e38270d0e84779170</t>
+  </si>
+  <si>
+    <t>a186665dd792aabe3f2cba60880e2d8f1b5017fb</t>
+  </si>
+  <si>
+    <t>util/</t>
+  </si>
+  <si>
+    <t>Eliot</t>
+  </si>
+  <si>
+    <t>Horowitz</t>
+  </si>
+  <si>
+    <t>grid/</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>bin/</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>Total LOC count</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +348,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -230,9 +389,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -248,6 +408,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Jan_2008_test_2" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -515,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1282"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4544,13 +4708,560 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
+    <col min="9" max="9" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="13" max="13" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="41.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="str">
+        <f>IFERROR(HLOOKUP(A2,$H4:BG$5,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <f>IFERROR(HLOOKUP($A2,$H$4:$S$5,2,FALSE),"")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D46" si="0">IFERROR(HLOOKUP($A3,$H$4:$S$5,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>32</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>8</v>
+      </c>
+      <c r="N5">
+        <v>12</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>10</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>0.107</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="C45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="C46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N49" s="2"/>
+    </row>
+    <row r="50" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N50" s="2"/>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N51" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commiting feburary changes start
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -367,12 +367,6 @@
     <t>// Use the same //=COUNTIF(I$2:J$24, "&gt;0.05") formula BUT when applying it, instead of dragging down as the others. You want to drag across the row.</t>
   </si>
   <si>
-    <t>This will get the columns to change. Then copy that then paste it with tabulation.</t>
-  </si>
-  <si>
-    <t>Since I had to manually insert columns for each contributor. I just copy paste and tabulate the contributor list here</t>
-  </si>
-  <si>
     <t>What I've been doing: Start with first author. -&gt; Copy paste all that falls under them within that range. Make sure I paste values not formulas. 
 Prooceed to next author. That way author names don't mixed up the hash</t>
   </si>
@@ -380,6 +374,12 @@
     <t xml:space="preserve">For me, this is the most tedious part of the aggregation of data.
 Once lines of code are here, you want o fill in all the blanks within the commits. Such that the percentages can line up with their commit's LOC to calculate column  F
 </t>
+  </si>
+  <si>
+    <t>Since I had to manually insert columns for each contributor. I just copy paste and transpose the contributor list here</t>
+  </si>
+  <si>
+    <t>This will get the columns to change. Then copy that then paste it with transposition.</t>
   </si>
 </sst>
 </file>
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1282"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,10 +813,10 @@
     </row>
     <row r="2" spans="1:17" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" t="e">
         <f>C2*E2</f>
@@ -841,7 +841,7 @@
       </c>
       <c r="N2" s="1"/>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P2" t="s">
         <v>42</v>
@@ -855,7 +855,7 @@
       <c r="G3" s="1"/>
       <c r="N3" s="1"/>
       <c r="P3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mid-way poitn of April data
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -19,6 +19,7 @@
     <definedName name="Jan_2008_test_2" localSheetId="1">'Raw Data Example'!$A$1:$C$46</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -352,9 +353,6 @@
     <t xml:space="preserve">Copy-Paste The Components Column. Then apply this formula =IF(D2="","",IF(COUNTIF($D2:D##endrange,D2)=1,D2,"")). It will clear up the components and leave only the unique ones. Then it becomes the tedious task of using ctrl+ - (or whatever mac uses) to shift the cells up. </t>
   </si>
   <si>
-    <t>/// Apply this formula to count major minor contributors per component.   =COUNTIF(User1Cell#:UserNCell#, "&lt;=0.05")-COUNTIF(User1Cell#:UserNCell#,"=0").</t>
-  </si>
-  <si>
     <t xml:space="preserve">  ///Same idea apply this formula: =COUNTIF(I2,J2, "&gt;0.05") //</t>
   </si>
   <si>
@@ -386,6 +384,10 @@
   </si>
   <si>
     <t>/// This the range of the author's components in their commits + loc. I usually record these on a separate notepad when I Do the initial cleaning up of authors from commit hashes row. =SUMPRODUCT(SUMIF($E$2:$E$409,I2,$F$2:$F$409))/J2</t>
+  </si>
+  <si>
+    <t>/// Apply this formula to count major minor contributors per component.   =COUNTIF(User1Cell#:UserNCell#, "&lt;=0.05")-COUNTIF(User1Cell#:UserNCell#,"=0"). Example
+=COUNTIF(J1:K2),"&lt;=0.05) - COUNTIF(J1:K2),"=0"</t>
   </si>
 </sst>
 </file>
@@ -763,6 +765,7 @@
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="43.42578125" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
     <col min="16" max="17" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -792,13 +795,13 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
         <v>34</v>
       </c>
       <c r="K1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L1" t="s">
         <v>5</v>
@@ -822,13 +825,13 @@
     </row>
     <row r="2" spans="1:18" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="F2" t="e">
-        <f>C2*E2</f>
+        <f t="shared" ref="F2:F7" si="0">C2*E2</f>
         <v>#VALUE!</v>
       </c>
       <c r="G2" s="1"/>
@@ -836,16 +839,16 @@
         <v>37</v>
       </c>
       <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
         <v>47</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>38</v>
-      </c>
-      <c r="M2" t="s">
-        <v>39</v>
       </c>
       <c r="N2">
         <f>MAX(J2:K2)</f>
@@ -853,21 +856,25 @@
       </c>
       <c r="O2" s="1"/>
       <c r="P2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F3">
-        <f t="shared" ref="F3:F7" si="0">C3*E3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G3" s="1"/>
+      <c r="N3">
+        <f>SUM(L2:M2)</f>
+        <v>0</v>
+      </c>
       <c r="O3" s="1"/>
       <c r="Q3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -4838,7 +4845,7 @@
   <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>